<commit_message>
Version 000 - Commit and Push na Branch correta
</commit_message>
<xml_diff>
--- a/dados_entrada.xlsx
+++ b/dados_entrada.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agcocorp-my.sharepoint.com/personal/rogerio_alves_agcocorp_com/Documents/00. ROGERIO ALVES_Documentos/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0281234d13572a04/Doutorado/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC1048C499D86CC85BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C213A30-B295-4D48-9ABE-49AFB981A121}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC1048C499D86CC85BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1854F0FB-1E1C-4397-9F00-E166F7E8B405}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,15 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>NOE</t>
-  </si>
-  <si>
-    <t>Org_Size</t>
-  </si>
-  <si>
-    <t>CC</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Estrutura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Níveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Membros_Nivel_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Membros_Nivel_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Membros_Nivel_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Numero_de_Departamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Membros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Org_Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CC</t>
   </si>
 </sst>
 </file>
@@ -69,9 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -89,6 +113,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -353,41 +381,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FA9A70-D076-430F-BB53-269DAF219FC8}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="G2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2000</v>
+      <c r="H2" s="1">
+        <v>100</v>
+      </c>
+      <c r="I2" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>